<commit_message>
Added pd.ewma method to functions. Added pooled scalars to Strategies.csv.
</commit_message>
<xml_diff>
--- a/SysTrade_Strategies.xlsx
+++ b/SysTrade_Strategies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="4520" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="2280" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,6 +405,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>5.19</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -419,6 +422,9 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>3.42</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -433,6 +439,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>2.38</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -444,6 +453,9 @@
       </c>
       <c r="D5">
         <v>1</v>
+      </c>
+      <c r="E5">
+        <v>11.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>